<commit_message>
Updated spring plan and readme
</commit_message>
<xml_diff>
--- a/SprintPlanning/Sprint 1/INFO-5139-Sprint Planning Meeting 1.0.xlsx
+++ b/SprintPlanning/Sprint 1/INFO-5139-Sprint Planning Meeting 1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DC64AC-40FB-4B53-A5C5-459FCF51755D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF1B196-4C3A-4095-BE07-876DB9D4A3E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Row #</t>
   </si>
@@ -270,15 +270,6 @@
     <t>FYF-1</t>
   </si>
   <si>
-    <t>FYF-2</t>
-  </si>
-  <si>
-    <t>FYF-10</t>
-  </si>
-  <si>
-    <t>FYF-13</t>
-  </si>
-  <si>
     <t>FYF-15</t>
   </si>
   <si>
@@ -288,27 +279,9 @@
     <t>Register in the app</t>
   </si>
   <si>
-    <t>Edit my profile</t>
-  </si>
-  <si>
-    <t>Fill in details about myself (Name, Gender, Age, College/University, Country of origin etc).</t>
-  </si>
-  <si>
     <t>Continue to creating my profile</t>
   </si>
   <si>
-    <t>Complete creating my profile</t>
-  </si>
-  <si>
-    <t>Maintain the accuracy of my personal</t>
-  </si>
-  <si>
-    <t>Create a post on my page</t>
-  </si>
-  <si>
-    <t>Share content with my friendlist</t>
-  </si>
-  <si>
     <t>Fast sign up with google account</t>
   </si>
   <si>
@@ -327,12 +300,6 @@
     <t>So people know what I am up to</t>
   </si>
   <si>
-    <t>Create a burger menu for mobile view</t>
-  </si>
-  <si>
-    <t>For people coming to site from mobiles</t>
-  </si>
-  <si>
     <t>FYF-33</t>
   </si>
   <si>
@@ -343,6 +310,12 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Create navigation bar</t>
+  </si>
+  <si>
+    <t>for easier navigation through the app</t>
   </si>
 </sst>
 </file>
@@ -565,17 +538,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>279622</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>182755</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>231309</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>106252</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1865B288-2656-417A-9DBA-6BD57037DB85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92B3B7B7-B257-46E5-8181-7D5792185D39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -592,7 +565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4838700"/>
-          <a:ext cx="24339772" cy="12755755"/>
+          <a:ext cx="19414659" cy="10583752"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -618,8 +591,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F24383E-81C1-48AA-B3CE-0A4651C21888}" name="Table13" displayName="Table13" ref="A4:F12" totalsRowShown="0">
-  <autoFilter ref="A4:F12" xr:uid="{6A4555D3-6CFC-4813-9C18-EEC3122BBE8B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F24383E-81C1-48AA-B3CE-0A4651C21888}" name="Table13" displayName="Table13" ref="A4:F9" totalsRowShown="0">
+  <autoFilter ref="A4:F9" xr:uid="{6A4555D3-6CFC-4813-9C18-EEC3122BBE8B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6C40B138-5F4F-4627-81B5-6CCFB7600CDB}" name="Row #"/>
     <tableColumn id="2" xr3:uid="{615EA2A2-FE7A-4D9C-9A42-7FA8DC77F155}" name="ID" dataDxfId="5"/>
@@ -946,7 +919,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A875DEB-4808-4559-B6A0-559BDD9EE661}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,16 +1125,16 @@
         <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5"/>
@@ -1169,45 +1142,45 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6"/>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7"/>
@@ -1215,22 +1188,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8"/>
@@ -1238,102 +1211,33 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
         <v>57</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" t="s">
-        <v>68</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9"/>
       <c r="K9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10"/>
-      <c r="K10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11"/>
-      <c r="K11"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12"/>
-      <c r="K12"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{D5E28F0E-7D6B-453A-BE92-021A9AAE5A60}">
       <formula1>"00, 01, 02, 03, 04, 05, 06, 07, 08, 09"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F12" xr:uid="{06EE48CD-350C-407D-8C90-E0AF6D94DA36}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F9" xr:uid="{06EE48CD-350C-407D-8C90-E0AF6D94DA36}">
       <formula1>"In Progress, On Hold, Testing, Done, Cancelled"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1350,7 +1254,7 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>